<commit_message>
export execl and statistical customerDebt
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -384,14 +384,20 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" customWidth="1" width="15"/>
+    <col min="1" max="1" customWidth="1" width="19"/>
     <col min="2" max="2" customWidth="1" width="14"/>
     <col min="3" max="3" customWidth="1" width="13"/>
-    <col min="4" max="4" customWidth="1" width="6"/>
-    <col min="5" max="5" customWidth="1" width="10"/>
-    <col min="6" max="6" customWidth="1" width="10"/>
+    <col min="4" max="4" customWidth="1" width="18"/>
+    <col min="5" max="5" customWidth="1" width="17"/>
+    <col min="6" max="6" customWidth="1" width="12"/>
   </cols>
   <sheetData>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>Danh sách Tuyến đương</v>
+      </c>
+    </row>
+    <row r="3"/>
     <row r="4">
       <c r="A4" t="str">
         <v>Tên tuyến đường</v>
@@ -417,10 +423,10 @@
         <v>Trần gia hiệu</v>
       </c>
       <c r="B5" s="1">
-        <v>44379.292129629626</v>
+        <v>44379.291712962964</v>
       </c>
       <c r="C5" s="1">
-        <v>44387.292129629626</v>
+        <v>44387.291712962964</v>
       </c>
       <c r="D5" t="str">
         <v>nhà xe phước sơn</v>
@@ -437,10 +443,10 @@
         <v>test</v>
       </c>
       <c r="B6" s="1">
-        <v>44378.292129629626</v>
+        <v>44378.291712962964</v>
       </c>
       <c r="C6" s="1">
-        <v>44379.292129629626</v>
+        <v>44379.291712962964</v>
       </c>
       <c r="D6" t="str">
         <v>test</v>
@@ -457,7 +463,7 @@
         <v>Bình định- Hội An</v>
       </c>
       <c r="B7" s="1">
-        <v>44406.292129629626</v>
+        <v>44406.291712962964</v>
       </c>
       <c r="D7" t="str">
         <v>Nhà xe Diêu Trì</v>
@@ -474,10 +480,10 @@
         <v>Bắc Nam</v>
       </c>
       <c r="B8" s="1">
-        <v>44378.292129629626</v>
+        <v>44378.291712962964</v>
       </c>
       <c r="C8" s="1">
-        <v>44378.292129629626</v>
+        <v>44378.291712962964</v>
       </c>
       <c r="D8" t="str">
         <v>nhà xe phước sơn</v>
@@ -494,7 +500,7 @@
         <v>Bac - Nam</v>
       </c>
       <c r="B9" s="1">
-        <v>35598.292129629626</v>
+        <v>35598.291712962964</v>
       </c>
       <c r="F9" t="str">
         <v>6546413</v>
@@ -505,10 +511,10 @@
         <v>Trần gia hiệu</v>
       </c>
       <c r="B10" s="1">
-        <v>44384.292129629626</v>
+        <v>44384.291712962964</v>
       </c>
       <c r="C10" s="1">
-        <v>44401.292129629626</v>
+        <v>44401.291712962964</v>
       </c>
       <c r="E10" t="str">
         <v>Nguyễn Văn A</v>
@@ -522,10 +528,10 @@
         <v>123</v>
       </c>
       <c r="B11" s="1">
-        <v>44378.292129629626</v>
+        <v>44378.291712962964</v>
       </c>
       <c r="C11" s="1">
-        <v>44393.292129629626</v>
+        <v>44393.291712962964</v>
       </c>
       <c r="D11" t="str">
         <v>garage</v>
@@ -542,7 +548,7 @@
         <v>Bac - Nam</v>
       </c>
       <c r="B12" s="1">
-        <v>35598.292129629626</v>
+        <v>35598.291712962964</v>
       </c>
       <c r="F12" t="str">
         <v>6546413</v>
@@ -553,7 +559,7 @@
         <v>Bac - Nam</v>
       </c>
       <c r="B13" s="1">
-        <v>35598.292129629626</v>
+        <v>35598.291712962964</v>
       </c>
       <c r="F13" t="str">
         <v>6546413</v>
@@ -564,7 +570,7 @@
         <v>Bac - Nam</v>
       </c>
       <c r="B14" s="1">
-        <v>35598.292129629626</v>
+        <v>35598.291712962964</v>
       </c>
       <c r="F14" t="str">
         <v>6546413</v>
@@ -575,7 +581,7 @@
         <v>Bac - Nam</v>
       </c>
       <c r="B15" s="1">
-        <v>35598.292129629626</v>
+        <v>35598.291712962964</v>
       </c>
       <c r="F15" t="str">
         <v>6546413</v>
@@ -586,7 +592,7 @@
         <v>Bac - Nam</v>
       </c>
       <c r="B16" s="1">
-        <v>35598.292129629626</v>
+        <v>35598.291712962964</v>
       </c>
       <c r="F16" t="str">
         <v>6546413</v>
@@ -597,7 +603,7 @@
         <v>Bac - Nam</v>
       </c>
       <c r="B17" s="1">
-        <v>35598.292129629626</v>
+        <v>35598.291712962964</v>
       </c>
       <c r="F17" t="str">
         <v>6546413</v>
@@ -608,7 +614,7 @@
         <v>Bac - Nam</v>
       </c>
       <c r="B18" s="1">
-        <v>35598.292129629626</v>
+        <v>35598.291712962964</v>
       </c>
       <c r="F18" t="str">
         <v>6546413</v>
@@ -619,7 +625,7 @@
         <v>Bac - Nam</v>
       </c>
       <c r="B19" s="1">
-        <v>35598.292129629626</v>
+        <v>35598.291712962964</v>
       </c>
       <c r="F19" t="str">
         <v>6546413</v>
@@ -630,7 +636,7 @@
         <v>Bac - Nam</v>
       </c>
       <c r="B20" s="1">
-        <v>35598.292129629626</v>
+        <v>35598.291712962964</v>
       </c>
       <c r="F20" t="str">
         <v>6546413</v>
@@ -641,7 +647,7 @@
         <v>Bac - Nam</v>
       </c>
       <c r="B21" s="1">
-        <v>35598.292129629626</v>
+        <v>35598.291712962964</v>
       </c>
       <c r="F21" t="str">
         <v>6546413</v>
@@ -652,7 +658,7 @@
         <v>Bac - Nam</v>
       </c>
       <c r="B22" s="1">
-        <v>35598.292129629626</v>
+        <v>35598.291712962964</v>
       </c>
       <c r="F22" t="str">
         <v>6546413</v>
@@ -663,7 +669,7 @@
         <v>Bac - Nam</v>
       </c>
       <c r="B23" s="1">
-        <v>35598.292129629626</v>
+        <v>35598.291712962964</v>
       </c>
       <c r="F23" t="str">
         <v>6546413</v>
@@ -674,7 +680,7 @@
         <v>Bac - Nam</v>
       </c>
       <c r="B24" s="1">
-        <v>35598.292129629626</v>
+        <v>35598.291712962964</v>
       </c>
       <c r="F24" t="str">
         <v>6546413</v>
@@ -685,7 +691,7 @@
         <v>Bac - Nam</v>
       </c>
       <c r="B25" s="1">
-        <v>35598.292129629626</v>
+        <v>35598.291712962964</v>
       </c>
       <c r="F25" t="str">
         <v>6546413</v>
@@ -696,7 +702,7 @@
         <v>Bac - Nam</v>
       </c>
       <c r="B26" s="1">
-        <v>35598.292129629626</v>
+        <v>35598.291712962964</v>
       </c>
       <c r="F26" t="str">
         <v>6546413</v>
@@ -707,7 +713,7 @@
         <v>Bac - Nam</v>
       </c>
       <c r="B27" s="1">
-        <v>35598.292129629626</v>
+        <v>35598.291712962964</v>
       </c>
       <c r="F27" t="str">
         <v>6546413</v>
@@ -718,7 +724,7 @@
         <v>Bac - Nam</v>
       </c>
       <c r="B28" s="1">
-        <v>35598.292129629626</v>
+        <v>35598.291712962964</v>
       </c>
       <c r="F28" t="str">
         <v>6546413</v>
@@ -729,7 +735,7 @@
         <v>Bac - Nam</v>
       </c>
       <c r="B29" s="1">
-        <v>35598.292129629626</v>
+        <v>35598.291712962964</v>
       </c>
       <c r="F29" t="str">
         <v>6546413</v>
@@ -740,7 +746,7 @@
         <v>Bac - Nam</v>
       </c>
       <c r="B30" s="1">
-        <v>35598.292129629626</v>
+        <v>35598.291712962964</v>
       </c>
       <c r="F30" t="str">
         <v>6546413</v>
@@ -751,7 +757,7 @@
         <v>Bac - Nam</v>
       </c>
       <c r="B31" s="1">
-        <v>35598.292129629626</v>
+        <v>35598.291712962964</v>
       </c>
       <c r="F31" t="str">
         <v>6546413</v>
@@ -762,7 +768,7 @@
         <v>Bac - Nam</v>
       </c>
       <c r="B32" s="1">
-        <v>35598.292129629626</v>
+        <v>35598.291712962964</v>
       </c>
       <c r="F32" t="str">
         <v>6546413</v>
@@ -773,7 +779,7 @@
         <v>Bac - Nam</v>
       </c>
       <c r="B33" s="1">
-        <v>35598.292129629626</v>
+        <v>35598.291712962964</v>
       </c>
       <c r="F33" t="str">
         <v>6546413</v>
@@ -784,7 +790,7 @@
         <v>Bac - Nam</v>
       </c>
       <c r="B34" s="1">
-        <v>35598.292129629626</v>
+        <v>35598.291712962964</v>
       </c>
       <c r="F34" t="str">
         <v>6546413</v>
@@ -795,7 +801,7 @@
         <v>Bac - Nam</v>
       </c>
       <c r="B35" s="1">
-        <v>35598.292129629626</v>
+        <v>35598.291712962964</v>
       </c>
       <c r="F35" t="str">
         <v>6546413</v>
@@ -806,7 +812,7 @@
         <v>Bac - Nam</v>
       </c>
       <c r="B36" s="1">
-        <v>35598.292129629626</v>
+        <v>35598.291712962964</v>
       </c>
       <c r="F36" t="str">
         <v>6546413</v>
@@ -817,7 +823,7 @@
         <v>Bac - Nam</v>
       </c>
       <c r="B37" s="1">
-        <v>35598.292129629626</v>
+        <v>35598.291712962964</v>
       </c>
       <c r="F37" t="str">
         <v>6546413</v>
@@ -828,7 +834,7 @@
         <v>Bac - Nam</v>
       </c>
       <c r="B38" s="1">
-        <v>35598.292129629626</v>
+        <v>35598.291712962964</v>
       </c>
       <c r="F38" t="str">
         <v>6546413</v>
@@ -839,7 +845,7 @@
         <v>Bac - Nam</v>
       </c>
       <c r="B39" s="1">
-        <v>35598.292129629626</v>
+        <v>35598.291712962964</v>
       </c>
       <c r="F39" t="str">
         <v>6546413</v>
@@ -850,7 +856,7 @@
         <v>Bac - Nam</v>
       </c>
       <c r="B40" s="1">
-        <v>35598.292129629626</v>
+        <v>35598.291712962964</v>
       </c>
       <c r="F40" t="str">
         <v>6546413</v>
@@ -861,7 +867,7 @@
         <v>Bac - Nam</v>
       </c>
       <c r="B41" s="1">
-        <v>35598.292129629626</v>
+        <v>35598.291712962964</v>
       </c>
       <c r="F41" t="str">
         <v>6546413</v>
@@ -872,7 +878,7 @@
         <v>Bac - Nam</v>
       </c>
       <c r="B42" s="1">
-        <v>35598.292129629626</v>
+        <v>35598.291712962964</v>
       </c>
       <c r="F42" t="str">
         <v>6546413</v>
@@ -883,7 +889,7 @@
         <v>Bac - Nam</v>
       </c>
       <c r="B43" s="1">
-        <v>35598.292129629626</v>
+        <v>35598.291712962964</v>
       </c>
       <c r="F43" t="str">
         <v>6546413</v>
@@ -894,7 +900,7 @@
         <v>Bac - Nam</v>
       </c>
       <c r="B44" s="1">
-        <v>35598.292129629626</v>
+        <v>35598.291712962964</v>
       </c>
       <c r="F44" t="str">
         <v>6546413</v>
@@ -905,7 +911,7 @@
         <v>Bac - Nam</v>
       </c>
       <c r="B45" s="1">
-        <v>35598.292129629626</v>
+        <v>35598.291712962964</v>
       </c>
       <c r="F45" t="str">
         <v>6546413</v>
@@ -916,7 +922,7 @@
         <v>Bac - Nam</v>
       </c>
       <c r="B46" s="1">
-        <v>35598.292129629626</v>
+        <v>35598.291712962964</v>
       </c>
       <c r="F46" t="str">
         <v>6546413</v>
@@ -924,6 +930,9 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:F46"/>
+  <mergeCells count="1">
+    <mergeCell ref="A2:F3"/>
+  </mergeCells>
   <ignoredErrors>
     <ignoredError numberStoredAsText="1" sqref="A1:F46"/>
   </ignoredErrors>

</xml_diff>